<commit_message>
Salva as predições do PCR (em dados com SG) no formato XLSX
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_sg.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_sg.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7484244397711524</v>
+        <v>0.7484244397710786</v>
       </c>
       <c r="D2" t="n">
-        <v>3.522632873055832</v>
+        <v>3.522632873056858</v>
       </c>
       <c r="E2" t="n">
-        <v>1.332766257947999</v>
+        <v>1.332766257948192</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7484244397711515</v>
+        <v>0.7484244397710785</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7389507385214874</v>
+        <v>0.7389507385214085</v>
       </c>
       <c r="D3" t="n">
-        <v>3.660697165498884</v>
+        <v>3.660697165500002</v>
       </c>
       <c r="E3" t="n">
-        <v>1.391741727524498</v>
+        <v>1.391741727524714</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7256671802024675</v>
+        <v>0.7256671802023824</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4635448637118251</v>
+        <v>0.4635448636911388</v>
       </c>
       <c r="D4" t="n">
-        <v>1.760382127916528</v>
+        <v>1.760382127984411</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2262934491824286</v>
+        <v>0.2262934491867918</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4635448637118252</v>
+        <v>0.4635448636911387</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.436002217671426</v>
+        <v>0.4360022176549992</v>
       </c>
       <c r="D5" t="n">
-        <v>1.849356069257175</v>
+        <v>1.849356069311443</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2410594429641713</v>
+        <v>0.2410594429673466</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3912517285220014</v>
+        <v>0.391251728505964</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5772997770821315</v>
+        <v>0.5772997770866438</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4741633712006582</v>
+        <v>0.4741633711955966</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3813924577539009</v>
+        <v>0.3813924577518653</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5772997770821313</v>
+        <v>0.5772997770866437</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5488035772330514</v>
+        <v>0.5488035772378166</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5033352602119229</v>
+        <v>0.5033352602065378</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4065888849456758</v>
+        <v>0.4065888849434595</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5196041133646374</v>
+        <v>0.5196041133698748</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5354074349808552</v>
+        <v>0.5354074349492267</v>
       </c>
       <c r="D8" t="n">
-        <v>238.3392061450005</v>
+        <v>238.3392061612262</v>
       </c>
       <c r="E8" t="n">
-        <v>70.0502114014421</v>
+        <v>70.05021140382655</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5354074349808553</v>
+        <v>0.5354074349492266</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5107983786302176</v>
+        <v>0.5107983785940841</v>
       </c>
       <c r="D9" t="n">
-        <v>250.4254245481042</v>
+        <v>250.4254245665182</v>
       </c>
       <c r="E9" t="n">
-        <v>74.60607576541469</v>
+        <v>74.60607576872304</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4730107589389639</v>
+        <v>0.4730107588922258</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6701777278136317</v>
+        <v>0.6701777278135673</v>
       </c>
       <c r="D10" t="n">
-        <v>5.06215316832957</v>
+        <v>5.062153168330556</v>
       </c>
       <c r="E10" t="n">
-        <v>1.847195534892265</v>
+        <v>1.84719553489245</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6701777278136321</v>
+        <v>0.6701777278135661</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.657997598066317</v>
+        <v>0.6579975980662301</v>
       </c>
       <c r="D11" t="n">
-        <v>5.258985402391192</v>
+        <v>5.258985402392566</v>
       </c>
       <c r="E11" t="n">
-        <v>1.932623687575767</v>
+        <v>1.932623687576084</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6389653910876961</v>
+        <v>0.6389653910875774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Salva as predições do PCR em dados com Savitzky-Golay Differentiation Filter
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_sg.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_sg.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7484244397710786</v>
+        <v>0.7484244397710726</v>
       </c>
       <c r="D2" t="n">
-        <v>3.522632873056858</v>
+        <v>3.52263287305694</v>
       </c>
       <c r="E2" t="n">
-        <v>1.332766257948192</v>
+        <v>1.332766257948208</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7484244397710785</v>
+        <v>0.7484244397710726</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7389507385214085</v>
+        <v>0.7389507385214021</v>
       </c>
       <c r="D3" t="n">
-        <v>3.660697165500002</v>
+        <v>3.660697165500093</v>
       </c>
       <c r="E3" t="n">
-        <v>1.391741727524714</v>
+        <v>1.391741727524732</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7256671802023824</v>
+        <v>0.7256671802023753</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4635448636911388</v>
+        <v>0.463544863547971</v>
       </c>
       <c r="D4" t="n">
-        <v>1.760382127984411</v>
+        <v>1.760382128454218</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2262934491867918</v>
+        <v>0.2262934492169881</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4635448636911387</v>
+        <v>0.4635448635479709</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4360022176549992</v>
+        <v>0.4360022175024897</v>
       </c>
       <c r="D5" t="n">
-        <v>1.849356069311443</v>
+        <v>1.84935606981256</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2410594429673466</v>
+        <v>0.2410594430005892</v>
       </c>
       <c r="F5" t="n">
-        <v>0.391251728505964</v>
+        <v>0.3912517283380692</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5772997770866438</v>
+        <v>0.5772997770802757</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4741633711955966</v>
+        <v>0.4741633712027403</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3813924577518653</v>
+        <v>0.3813924577547379</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5772997770866437</v>
+        <v>0.577299777080276</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5488035772378166</v>
+        <v>0.5488035772307361</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5033352602065378</v>
+        <v>0.503335260214279</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4065888849434595</v>
+        <v>0.4065888849461675</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5196041133698748</v>
+        <v>0.5196041133634757</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5354074349492267</v>
+        <v>0.5354074349440815</v>
       </c>
       <c r="D8" t="n">
-        <v>238.3392061612262</v>
+        <v>238.3392061638659</v>
       </c>
       <c r="E8" t="n">
-        <v>70.05021140382655</v>
+        <v>70.05021140421445</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5354074349492266</v>
+        <v>0.5354074349440814</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5107983785940841</v>
+        <v>0.5107983785875997</v>
       </c>
       <c r="D9" t="n">
-        <v>250.4254245665182</v>
+        <v>250.4254245697775</v>
       </c>
       <c r="E9" t="n">
-        <v>74.60607576872304</v>
+        <v>74.60607576946802</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4730107588922258</v>
+        <v>0.4730107588817013</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6701777278135673</v>
+        <v>0.6701777278163675</v>
       </c>
       <c r="D10" t="n">
-        <v>5.062153168330556</v>
+        <v>5.06215316828758</v>
       </c>
       <c r="E10" t="n">
-        <v>1.84719553489245</v>
+        <v>1.847195534884605</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6701777278135661</v>
+        <v>0.6701777278163674</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6579975980662301</v>
+        <v>0.6579975980689318</v>
       </c>
       <c r="D11" t="n">
-        <v>5.258985402392566</v>
+        <v>5.258985402350601</v>
       </c>
       <c r="E11" t="n">
-        <v>1.932623687576084</v>
+        <v>1.932623687568715</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6389653910875774</v>
+        <v>0.6389653910903306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adiciona arquivos com informações do plot do PCR com filtro SG
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_sg.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_sg.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7484244397710726</v>
+        <v>0.7652488218523669</v>
       </c>
       <c r="D2" t="n">
-        <v>3.52263287305694</v>
+        <v>3.287053068188353</v>
       </c>
       <c r="E2" t="n">
-        <v>1.332766257948208</v>
+        <v>1.287430089285444</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7484244397710726</v>
+        <v>0.7652488218523665</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7389507385214021</v>
+        <v>0.7521081881793897</v>
       </c>
       <c r="D3" t="n">
-        <v>3.660697165500093</v>
+        <v>3.482316337766491</v>
       </c>
       <c r="E3" t="n">
-        <v>1.391741727524732</v>
+        <v>1.367345623478399</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7256671802023753</v>
+        <v>0.7352005490771096</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.463544863547971</v>
+        <v>0.4688054747003463</v>
       </c>
       <c r="D4" t="n">
-        <v>1.760382128454218</v>
+        <v>1.743119387866745</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2262934492169881</v>
+        <v>0.2251811710404823</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4635448635479709</v>
+        <v>0.4688054747003464</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4360022175024897</v>
+        <v>0.4383441132901364</v>
       </c>
       <c r="D5" t="n">
-        <v>1.84935606981256</v>
+        <v>1.841827598857237</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2410594430005892</v>
+        <v>0.2412183778558042</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3912517283380692</v>
+        <v>0.3904487462008647</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5772997770802757</v>
+        <v>0.5529044951640609</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4741633712027403</v>
+        <v>0.5015287438418512</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3813924577547379</v>
+        <v>0.3922437331892626</v>
       </c>
       <c r="F6" t="n">
-        <v>0.577299777080276</v>
+        <v>0.5529044951640609</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5488035772307361</v>
+        <v>0.5293487356155337</v>
       </c>
       <c r="D7" t="n">
-        <v>0.503335260214279</v>
+        <v>0.5249115170629832</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4065888849461675</v>
+        <v>0.4138859651466079</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5196041133634757</v>
+        <v>0.5022059794685393</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5354074349440815</v>
+        <v>0.549793735567308</v>
       </c>
       <c r="D8" t="n">
-        <v>238.3392061638659</v>
+        <v>230.9589342265355</v>
       </c>
       <c r="E8" t="n">
-        <v>70.05021140421445</v>
+        <v>68.95711596322518</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5354074349440814</v>
+        <v>0.5497937355673072</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5107983785875997</v>
+        <v>0.5215083906738172</v>
       </c>
       <c r="D9" t="n">
-        <v>250.4254245697775</v>
+        <v>244.9523546852538</v>
       </c>
       <c r="E9" t="n">
-        <v>74.60607576946802</v>
+        <v>74.60437642749604</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4730107588817013</v>
+        <v>0.4730347656325711</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6701777278163675</v>
+        <v>0.6704659607956678</v>
       </c>
       <c r="D10" t="n">
-        <v>5.06215316828758</v>
+        <v>5.057729332748186</v>
       </c>
       <c r="E10" t="n">
-        <v>1.847195534884605</v>
+        <v>1.846388222750611</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6701777278163674</v>
+        <v>0.6704659607956677</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6579975980689318</v>
+        <v>0.6562443076201127</v>
       </c>
       <c r="D11" t="n">
-        <v>5.258985402350601</v>
+        <v>5.286829133673952</v>
       </c>
       <c r="E11" t="n">
-        <v>1.932623687568715</v>
+        <v>1.94719964562402</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6389653910903306</v>
+        <v>0.6334989672791522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>